<commit_message>
add: add cheat sheet (#3)
</commit_message>
<xml_diff>
--- a/GroupCase/Group3_Case Materials/Hola-Kola_Case_PCF_Answer.xlsx
+++ b/GroupCase/Group3_Case Materials/Hola-Kola_Case_PCF_Answer.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBAB70F-4081-2F4F-9BD9-B78BA5F97509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5A7E73-DACC-514F-A042-D49690651D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="2" r:id="rId1"/>
@@ -577,62 +577,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1244390</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>167644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>521292</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>65865</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3218DEDE-0166-584D-B6F9-D88B729F38B1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:alphaModFix amt="20000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1244390" y="3145575"/>
-          <a:ext cx="5955350" cy="5503738"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -956,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1006,7 +950,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="37">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>2</v>
@@ -1321,19 +1265,19 @@
       </c>
       <c r="D29" s="47">
         <f t="shared" ref="D29:G29" si="1">(12 * $C$5 * (1+$C$6)^D18 * $C$7 * (1+$C$8)^D18) / 365 * $H$9</f>
-        <v>4438356.1643835614</v>
+        <v>4660273.9726027399</v>
       </c>
       <c r="E29" s="47">
         <f t="shared" si="1"/>
-        <v>4438356.1643835614</v>
+        <v>4893287.6712328773</v>
       </c>
       <c r="F29" s="47">
         <f t="shared" si="1"/>
-        <v>4438356.1643835614</v>
+        <v>5137952.0547945211</v>
       </c>
       <c r="G29" s="47">
         <f t="shared" si="1"/>
-        <v>4438356.1643835614</v>
+        <v>5394849.6575342473</v>
       </c>
       <c r="H29" s="47">
         <v>0</v>
@@ -1349,19 +1293,19 @@
       </c>
       <c r="D30" s="47">
         <f t="shared" ref="D30:G30" si="2">$C$5 * (1+$C$6)^D18 * $C$9 * (1+$C$10)^D18</f>
-        <v>1080000</v>
+        <v>1134000</v>
       </c>
       <c r="E30" s="47">
         <f t="shared" si="2"/>
-        <v>1080000</v>
+        <v>1190700</v>
       </c>
       <c r="F30" s="47">
         <f t="shared" si="2"/>
-        <v>1080000</v>
+        <v>1250235.0000000002</v>
       </c>
       <c r="G30" s="47">
         <f t="shared" si="2"/>
-        <v>1080000</v>
+        <v>1312746.75</v>
       </c>
       <c r="H30" s="47">
         <v>0</v>
@@ -1377,19 +1321,19 @@
       </c>
       <c r="D31" s="51">
         <f t="shared" ref="D31:G31" si="3">-(12 * $C$5 * (1+$C$6)^D18 * $C$9 * (1+$C$10)^D18) / 365 * $H$10</f>
-        <v>-1278246.5753424659</v>
+        <v>-1342158.9041095888</v>
       </c>
       <c r="E31" s="51">
         <f t="shared" si="3"/>
-        <v>-1278246.5753424659</v>
+        <v>-1409266.8493150687</v>
       </c>
       <c r="F31" s="51">
         <f t="shared" si="3"/>
-        <v>-1278246.5753424659</v>
+        <v>-1479730.1917808221</v>
       </c>
       <c r="G31" s="51">
         <f t="shared" si="3"/>
-        <v>-1278246.5753424659</v>
+        <v>-1553716.701369863</v>
       </c>
       <c r="H31" s="51">
         <v>0</v>
@@ -1402,19 +1346,19 @@
       </c>
       <c r="D32" s="15">
         <f t="shared" ref="D32:H32" si="4">SUM(D29:D31)</f>
-        <v>4240109.5890410952</v>
+        <v>4452115.0684931511</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="4"/>
-        <v>4240109.5890410952</v>
+        <v>4674720.8219178086</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="4"/>
-        <v>4240109.5890410952</v>
+        <v>4908456.8630136987</v>
       </c>
       <c r="G32" s="15">
         <f t="shared" si="4"/>
-        <v>4240109.5890410952</v>
+        <v>5153879.7061643843</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="4"/>
@@ -1440,23 +1384,23 @@
       </c>
       <c r="D34" s="20">
         <f t="shared" ref="D34:H34" si="5">-(D32-C32)</f>
-        <v>0</v>
+        <v>-212005.47945205588</v>
       </c>
       <c r="E34" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-222605.75342465751</v>
       </c>
       <c r="F34" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-233736.0410958901</v>
       </c>
       <c r="G34" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-245422.84315068554</v>
       </c>
       <c r="H34" s="20">
         <f t="shared" si="5"/>
-        <v>4240109.5890410952</v>
+        <v>5153879.7061643843</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
@@ -1469,19 +1413,19 @@
       </c>
       <c r="E36" s="48">
         <f t="shared" ref="E36:H36" si="6">12 * $C$5 * (1+$C$6)^D18</f>
-        <v>7200000</v>
+        <v>7560000</v>
       </c>
       <c r="F36" s="48">
         <f t="shared" si="6"/>
-        <v>7200000</v>
+        <v>7938000</v>
       </c>
       <c r="G36" s="48">
         <f t="shared" si="6"/>
-        <v>7200000</v>
+        <v>8334900.0000000009</v>
       </c>
       <c r="H36" s="48">
         <f t="shared" si="6"/>
-        <v>7200000</v>
+        <v>8751645</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
@@ -1494,19 +1438,19 @@
       </c>
       <c r="E37" s="15">
         <f t="shared" ref="E37:H37" si="7">E36 * $C$7 * (1+$C$8)^E18</f>
-        <v>36000000</v>
+        <v>37800000</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="7"/>
-        <v>36000000</v>
+        <v>39690000</v>
       </c>
       <c r="G37" s="15">
         <f t="shared" si="7"/>
-        <v>36000000</v>
+        <v>41674500.000000007</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="7"/>
-        <v>36000000</v>
+        <v>43758225</v>
       </c>
       <c r="I37" s="21"/>
     </row>
@@ -1525,19 +1469,19 @@
       </c>
       <c r="E40" s="48">
         <f t="shared" ref="E40:H40" si="8">-(12 * $C$5 * (1+$C$6)^D18 * $C$9 * (1+$C$10)^D18)</f>
-        <v>-12960000</v>
+        <v>-13608000</v>
       </c>
       <c r="F40" s="48">
         <f t="shared" si="8"/>
-        <v>-12960000</v>
+        <v>-14288400</v>
       </c>
       <c r="G40" s="48">
         <f t="shared" si="8"/>
-        <v>-12960000</v>
+        <v>-15002820.000000002</v>
       </c>
       <c r="H40" s="48">
         <f t="shared" si="8"/>
-        <v>-12960000</v>
+        <v>-15752961</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
@@ -1670,19 +1614,19 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ref="E46:G46" si="13">-E37*$H$7</f>
-        <v>-360000</v>
+        <v>-378000</v>
       </c>
       <c r="F46" s="52">
         <f t="shared" si="13"/>
-        <v>-360000</v>
+        <v>-396900</v>
       </c>
       <c r="G46" s="52">
         <f t="shared" si="13"/>
-        <v>-360000</v>
+        <v>-416745.00000000006</v>
       </c>
       <c r="H46" s="52">
         <f>-H37*$H$7</f>
-        <v>-360000</v>
+        <v>-437582.25</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
@@ -1695,19 +1639,19 @@
       </c>
       <c r="E47" s="15">
         <f t="shared" ref="E47:H47" si="14">SUM(E40:E46)</f>
-        <v>-26440000</v>
+        <v>-27106000</v>
       </c>
       <c r="F47" s="15">
         <f t="shared" si="14"/>
-        <v>-26440000</v>
+        <v>-27805300</v>
       </c>
       <c r="G47" s="15">
         <f t="shared" si="14"/>
-        <v>-26440000</v>
+        <v>-28539565</v>
       </c>
       <c r="H47" s="15">
         <f t="shared" si="14"/>
-        <v>-26440000</v>
+        <v>-29310543.25</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
@@ -1727,19 +1671,19 @@
       </c>
       <c r="E49" s="15">
         <f t="shared" ref="E49:H49" si="15">E37+E47</f>
-        <v>9560000</v>
+        <v>10694000</v>
       </c>
       <c r="F49" s="15">
         <f t="shared" si="15"/>
-        <v>9560000</v>
+        <v>11884700</v>
       </c>
       <c r="G49" s="15">
         <f t="shared" si="15"/>
-        <v>9560000</v>
+        <v>13134935.000000007</v>
       </c>
       <c r="H49" s="15">
         <f t="shared" si="15"/>
-        <v>9560000</v>
+        <v>14447681.75</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.15">
@@ -1772,19 +1716,19 @@
       </c>
       <c r="E51" s="15">
         <f t="shared" ref="E51:H51" si="16">-E49*$H$13</f>
-        <v>-2868000</v>
+        <v>-3208200</v>
       </c>
       <c r="F51" s="15">
         <f t="shared" si="16"/>
-        <v>-2868000</v>
+        <v>-3565410</v>
       </c>
       <c r="G51" s="15">
         <f t="shared" si="16"/>
-        <v>-2868000</v>
+        <v>-3940480.5000000019</v>
       </c>
       <c r="H51" s="15">
         <f t="shared" si="16"/>
-        <v>-2868000</v>
+        <v>-4334304.5249999994</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
@@ -1797,19 +1741,19 @@
       </c>
       <c r="E53" s="15">
         <f t="shared" ref="E53:H53" si="17">E49+E51</f>
-        <v>6692000</v>
+        <v>7485800</v>
       </c>
       <c r="F53" s="15">
         <f t="shared" si="17"/>
-        <v>6692000</v>
+        <v>8319290</v>
       </c>
       <c r="G53" s="15">
         <f t="shared" si="17"/>
-        <v>6692000</v>
+        <v>9194454.5000000056</v>
       </c>
       <c r="H53" s="15">
         <f t="shared" si="17"/>
-        <v>6692000</v>
+        <v>10113377.225000001</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
@@ -1886,19 +1830,19 @@
       </c>
       <c r="E58" s="20">
         <f t="shared" ref="E58:H58" si="20">E53+E56+E57</f>
-        <v>15892000</v>
+        <v>16685800</v>
       </c>
       <c r="F58" s="20">
         <f t="shared" si="20"/>
-        <v>15892000</v>
+        <v>17519290</v>
       </c>
       <c r="G58" s="20">
         <f t="shared" si="20"/>
-        <v>15892000</v>
+        <v>18394454.500000007</v>
       </c>
       <c r="H58" s="20">
         <f t="shared" si="20"/>
-        <v>15892000</v>
+        <v>19313377.225000001</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.15">
@@ -1912,23 +1856,23 @@
       </c>
       <c r="D60" s="20">
         <f>D26+D34+D58</f>
-        <v>15892000</v>
+        <v>15679994.520547945</v>
       </c>
       <c r="E60" s="20">
         <f t="shared" ref="E60:H60" si="21">E26+E34+E58</f>
-        <v>15892000</v>
+        <v>16463194.246575342</v>
       </c>
       <c r="F60" s="20">
         <f t="shared" si="21"/>
-        <v>15892000</v>
+        <v>17285553.95890411</v>
       </c>
       <c r="G60" s="20">
         <f t="shared" si="21"/>
-        <v>15892000</v>
+        <v>18149031.656849321</v>
       </c>
       <c r="H60" s="20">
         <f t="shared" si="21"/>
-        <v>22932109.589041095</v>
+        <v>27267256.931164384</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.15">
@@ -1941,23 +1885,23 @@
       </c>
       <c r="D61" s="49">
         <f>C61+D60</f>
-        <v>-38348109.589041099</v>
+        <v>-38560115.068493158</v>
       </c>
       <c r="E61" s="49">
         <f>D61+E60</f>
-        <v>-22456109.589041099</v>
+        <v>-22096920.821917817</v>
       </c>
       <c r="F61" s="49">
         <f>E61+F60</f>
-        <v>-6564109.589041099</v>
+        <v>-4811366.8630137071</v>
       </c>
       <c r="G61" s="49">
         <f>F61+G60</f>
-        <v>9327890.410958901</v>
+        <v>13337664.793835614</v>
       </c>
       <c r="H61" s="49">
         <f>G61+H60</f>
-        <v>32259999.999999996</v>
+        <v>40604921.724999994</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.15">
@@ -1970,23 +1914,23 @@
       </c>
       <c r="D63" s="49">
         <f t="shared" si="22"/>
-        <v>13445008.460236887</v>
+        <v>13265646.802494032</v>
       </c>
       <c r="E63" s="49">
         <f t="shared" si="22"/>
-        <v>11374795.651638653</v>
+        <v>11783631.407502372</v>
       </c>
       <c r="F63" s="49">
         <f t="shared" si="22"/>
-        <v>9623346.574990401</v>
+        <v>10467208.437404457</v>
       </c>
       <c r="G63" s="49">
         <f t="shared" si="22"/>
-        <v>8141579.1666585468</v>
+        <v>9297871.7614164911</v>
       </c>
       <c r="H63" s="49">
         <f>H60/(1+$H$12)^H18</f>
-        <v>9939318.9178002533</v>
+        <v>11818274.354573885</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.15">
@@ -1999,23 +1943,23 @@
       </c>
       <c r="D64" s="49">
         <f>C64+D63</f>
-        <v>-40795101.128804214</v>
+        <v>-40974462.786547065</v>
       </c>
       <c r="E64" s="49">
         <f t="shared" ref="E64:H64" si="23">D64+E63</f>
-        <v>-29420305.477165561</v>
+        <v>-29190831.379044693</v>
       </c>
       <c r="F64" s="49">
         <f t="shared" si="23"/>
-        <v>-19796958.902175158</v>
+        <v>-18723622.941640235</v>
       </c>
       <c r="G64" s="49">
         <f t="shared" si="23"/>
-        <v>-11655379.735516611</v>
+        <v>-9425751.1802237444</v>
       </c>
       <c r="H64" s="49">
         <f t="shared" si="23"/>
-        <v>-1716060.8177163582</v>
+        <v>2392523.1743501406</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.15">
@@ -2025,7 +1969,7 @@
       <c r="B66" s="24"/>
       <c r="C66" s="50">
         <f>C60+NPV($H$12,D60:H60)</f>
-        <v>-1716060.8177163675</v>
+        <v>2392523.174350135</v>
       </c>
       <c r="D66" s="15"/>
     </row>
@@ -2036,7 +1980,7 @@
       <c r="B67" s="26"/>
       <c r="C67" s="27">
         <f>IRR(C60:H60)</f>
-        <v>0.16858705103377836</v>
+        <v>0.19979255448030542</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.15">
@@ -2046,7 +1990,7 @@
       <c r="B68" s="26"/>
       <c r="C68" s="28">
         <f>F18 - F61/G60</f>
-        <v>3.4130449024063112</v>
+        <v>3.265103227212562</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.15">
@@ -2065,7 +2009,7 @@
       <c r="B70" s="31"/>
       <c r="C70" s="32">
         <f>-NPV($H$12,D60:H60)/C60</f>
-        <v>0.96836177451118044</v>
+        <v>1.0441098514084406</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.15">
@@ -2082,6 +2026,5 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: finish reviews (#3)
</commit_message>
<xml_diff>
--- a/GroupCase/Group3_Case Materials/Hola-Kola_Case_PCF_Answer.xlsx
+++ b/GroupCase/Group3_Case Materials/Hola-Kola_Case_PCF_Answer.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5A7E73-DACC-514F-A042-D49690651D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25F660B-6EC0-C746-BFB9-3CA177AC11A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="37">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>2</v>
@@ -1265,19 +1265,19 @@
       </c>
       <c r="D29" s="47">
         <f t="shared" ref="D29:G29" si="1">(12 * $C$5 * (1+$C$6)^D18 * $C$7 * (1+$C$8)^D18) / 365 * $H$9</f>
-        <v>4660273.9726027399</v>
+        <v>4438356.1643835614</v>
       </c>
       <c r="E29" s="47">
         <f t="shared" si="1"/>
-        <v>4893287.6712328773</v>
+        <v>4438356.1643835614</v>
       </c>
       <c r="F29" s="47">
         <f t="shared" si="1"/>
-        <v>5137952.0547945211</v>
+        <v>4438356.1643835614</v>
       </c>
       <c r="G29" s="47">
         <f t="shared" si="1"/>
-        <v>5394849.6575342473</v>
+        <v>4438356.1643835614</v>
       </c>
       <c r="H29" s="47">
         <v>0</v>
@@ -1293,19 +1293,19 @@
       </c>
       <c r="D30" s="47">
         <f t="shared" ref="D30:G30" si="2">$C$5 * (1+$C$6)^D18 * $C$9 * (1+$C$10)^D18</f>
-        <v>1134000</v>
+        <v>1080000</v>
       </c>
       <c r="E30" s="47">
         <f t="shared" si="2"/>
-        <v>1190700</v>
+        <v>1080000</v>
       </c>
       <c r="F30" s="47">
         <f t="shared" si="2"/>
-        <v>1250235.0000000002</v>
+        <v>1080000</v>
       </c>
       <c r="G30" s="47">
         <f t="shared" si="2"/>
-        <v>1312746.75</v>
+        <v>1080000</v>
       </c>
       <c r="H30" s="47">
         <v>0</v>
@@ -1321,19 +1321,19 @@
       </c>
       <c r="D31" s="51">
         <f t="shared" ref="D31:G31" si="3">-(12 * $C$5 * (1+$C$6)^D18 * $C$9 * (1+$C$10)^D18) / 365 * $H$10</f>
-        <v>-1342158.9041095888</v>
+        <v>-1278246.5753424659</v>
       </c>
       <c r="E31" s="51">
         <f t="shared" si="3"/>
-        <v>-1409266.8493150687</v>
+        <v>-1278246.5753424659</v>
       </c>
       <c r="F31" s="51">
         <f t="shared" si="3"/>
-        <v>-1479730.1917808221</v>
+        <v>-1278246.5753424659</v>
       </c>
       <c r="G31" s="51">
         <f t="shared" si="3"/>
-        <v>-1553716.701369863</v>
+        <v>-1278246.5753424659</v>
       </c>
       <c r="H31" s="51">
         <v>0</v>
@@ -1346,19 +1346,19 @@
       </c>
       <c r="D32" s="15">
         <f t="shared" ref="D32:H32" si="4">SUM(D29:D31)</f>
-        <v>4452115.0684931511</v>
+        <v>4240109.5890410952</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="4"/>
-        <v>4674720.8219178086</v>
+        <v>4240109.5890410952</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="4"/>
-        <v>4908456.8630136987</v>
+        <v>4240109.5890410952</v>
       </c>
       <c r="G32" s="15">
         <f t="shared" si="4"/>
-        <v>5153879.7061643843</v>
+        <v>4240109.5890410952</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="4"/>
@@ -1384,23 +1384,23 @@
       </c>
       <c r="D34" s="20">
         <f t="shared" ref="D34:H34" si="5">-(D32-C32)</f>
-        <v>-212005.47945205588</v>
+        <v>0</v>
       </c>
       <c r="E34" s="20">
         <f t="shared" si="5"/>
-        <v>-222605.75342465751</v>
+        <v>0</v>
       </c>
       <c r="F34" s="20">
         <f t="shared" si="5"/>
-        <v>-233736.0410958901</v>
+        <v>0</v>
       </c>
       <c r="G34" s="20">
         <f t="shared" si="5"/>
-        <v>-245422.84315068554</v>
+        <v>0</v>
       </c>
       <c r="H34" s="20">
         <f t="shared" si="5"/>
-        <v>5153879.7061643843</v>
+        <v>4240109.5890410952</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
@@ -1413,19 +1413,19 @@
       </c>
       <c r="E36" s="48">
         <f t="shared" ref="E36:H36" si="6">12 * $C$5 * (1+$C$6)^D18</f>
-        <v>7560000</v>
+        <v>7200000</v>
       </c>
       <c r="F36" s="48">
         <f t="shared" si="6"/>
-        <v>7938000</v>
+        <v>7200000</v>
       </c>
       <c r="G36" s="48">
         <f t="shared" si="6"/>
-        <v>8334900.0000000009</v>
+        <v>7200000</v>
       </c>
       <c r="H36" s="48">
         <f t="shared" si="6"/>
-        <v>8751645</v>
+        <v>7200000</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
@@ -1438,19 +1438,19 @@
       </c>
       <c r="E37" s="15">
         <f t="shared" ref="E37:H37" si="7">E36 * $C$7 * (1+$C$8)^E18</f>
-        <v>37800000</v>
+        <v>36000000</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="7"/>
-        <v>39690000</v>
+        <v>36000000</v>
       </c>
       <c r="G37" s="15">
         <f t="shared" si="7"/>
-        <v>41674500.000000007</v>
+        <v>36000000</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="7"/>
-        <v>43758225</v>
+        <v>36000000</v>
       </c>
       <c r="I37" s="21"/>
     </row>
@@ -1469,19 +1469,19 @@
       </c>
       <c r="E40" s="48">
         <f t="shared" ref="E40:H40" si="8">-(12 * $C$5 * (1+$C$6)^D18 * $C$9 * (1+$C$10)^D18)</f>
-        <v>-13608000</v>
+        <v>-12960000</v>
       </c>
       <c r="F40" s="48">
         <f t="shared" si="8"/>
-        <v>-14288400</v>
+        <v>-12960000</v>
       </c>
       <c r="G40" s="48">
         <f t="shared" si="8"/>
-        <v>-15002820.000000002</v>
+        <v>-12960000</v>
       </c>
       <c r="H40" s="48">
         <f t="shared" si="8"/>
-        <v>-15752961</v>
+        <v>-12960000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
@@ -1614,19 +1614,19 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ref="E46:G46" si="13">-E37*$H$7</f>
-        <v>-378000</v>
+        <v>-360000</v>
       </c>
       <c r="F46" s="52">
         <f t="shared" si="13"/>
-        <v>-396900</v>
+        <v>-360000</v>
       </c>
       <c r="G46" s="52">
         <f t="shared" si="13"/>
-        <v>-416745.00000000006</v>
+        <v>-360000</v>
       </c>
       <c r="H46" s="52">
         <f>-H37*$H$7</f>
-        <v>-437582.25</v>
+        <v>-360000</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
@@ -1639,19 +1639,19 @@
       </c>
       <c r="E47" s="15">
         <f t="shared" ref="E47:H47" si="14">SUM(E40:E46)</f>
-        <v>-27106000</v>
+        <v>-26440000</v>
       </c>
       <c r="F47" s="15">
         <f t="shared" si="14"/>
-        <v>-27805300</v>
+        <v>-26440000</v>
       </c>
       <c r="G47" s="15">
         <f t="shared" si="14"/>
-        <v>-28539565</v>
+        <v>-26440000</v>
       </c>
       <c r="H47" s="15">
         <f t="shared" si="14"/>
-        <v>-29310543.25</v>
+        <v>-26440000</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
@@ -1671,19 +1671,19 @@
       </c>
       <c r="E49" s="15">
         <f t="shared" ref="E49:H49" si="15">E37+E47</f>
-        <v>10694000</v>
+        <v>9560000</v>
       </c>
       <c r="F49" s="15">
         <f t="shared" si="15"/>
-        <v>11884700</v>
+        <v>9560000</v>
       </c>
       <c r="G49" s="15">
         <f t="shared" si="15"/>
-        <v>13134935.000000007</v>
+        <v>9560000</v>
       </c>
       <c r="H49" s="15">
         <f t="shared" si="15"/>
-        <v>14447681.75</v>
+        <v>9560000</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.15">
@@ -1716,19 +1716,19 @@
       </c>
       <c r="E51" s="15">
         <f t="shared" ref="E51:H51" si="16">-E49*$H$13</f>
-        <v>-3208200</v>
+        <v>-2868000</v>
       </c>
       <c r="F51" s="15">
         <f t="shared" si="16"/>
-        <v>-3565410</v>
+        <v>-2868000</v>
       </c>
       <c r="G51" s="15">
         <f t="shared" si="16"/>
-        <v>-3940480.5000000019</v>
+        <v>-2868000</v>
       </c>
       <c r="H51" s="15">
         <f t="shared" si="16"/>
-        <v>-4334304.5249999994</v>
+        <v>-2868000</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
@@ -1741,19 +1741,19 @@
       </c>
       <c r="E53" s="15">
         <f t="shared" ref="E53:H53" si="17">E49+E51</f>
-        <v>7485800</v>
+        <v>6692000</v>
       </c>
       <c r="F53" s="15">
         <f t="shared" si="17"/>
-        <v>8319290</v>
+        <v>6692000</v>
       </c>
       <c r="G53" s="15">
         <f t="shared" si="17"/>
-        <v>9194454.5000000056</v>
+        <v>6692000</v>
       </c>
       <c r="H53" s="15">
         <f t="shared" si="17"/>
-        <v>10113377.225000001</v>
+        <v>6692000</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
@@ -1830,19 +1830,19 @@
       </c>
       <c r="E58" s="20">
         <f t="shared" ref="E58:H58" si="20">E53+E56+E57</f>
-        <v>16685800</v>
+        <v>15892000</v>
       </c>
       <c r="F58" s="20">
         <f t="shared" si="20"/>
-        <v>17519290</v>
+        <v>15892000</v>
       </c>
       <c r="G58" s="20">
         <f t="shared" si="20"/>
-        <v>18394454.500000007</v>
+        <v>15892000</v>
       </c>
       <c r="H58" s="20">
-        <f t="shared" si="20"/>
-        <v>19313377.225000001</v>
+        <f>H53+H56+H57</f>
+        <v>15892000</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.15">
@@ -1856,23 +1856,23 @@
       </c>
       <c r="D60" s="20">
         <f>D26+D34+D58</f>
-        <v>15679994.520547945</v>
+        <v>15892000</v>
       </c>
       <c r="E60" s="20">
         <f t="shared" ref="E60:H60" si="21">E26+E34+E58</f>
-        <v>16463194.246575342</v>
+        <v>15892000</v>
       </c>
       <c r="F60" s="20">
         <f t="shared" si="21"/>
-        <v>17285553.95890411</v>
+        <v>15892000</v>
       </c>
       <c r="G60" s="20">
         <f t="shared" si="21"/>
-        <v>18149031.656849321</v>
+        <v>15892000</v>
       </c>
       <c r="H60" s="20">
-        <f t="shared" si="21"/>
-        <v>27267256.931164384</v>
+        <f>H26+H34+H58</f>
+        <v>22932109.589041095</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.15">
@@ -1885,23 +1885,23 @@
       </c>
       <c r="D61" s="49">
         <f>C61+D60</f>
-        <v>-38560115.068493158</v>
+        <v>-38348109.589041099</v>
       </c>
       <c r="E61" s="49">
         <f>D61+E60</f>
-        <v>-22096920.821917817</v>
+        <v>-22456109.589041099</v>
       </c>
       <c r="F61" s="49">
         <f>E61+F60</f>
-        <v>-4811366.8630137071</v>
+        <v>-6564109.589041099</v>
       </c>
       <c r="G61" s="49">
         <f>F61+G60</f>
-        <v>13337664.793835614</v>
+        <v>9327890.410958901</v>
       </c>
       <c r="H61" s="49">
         <f>G61+H60</f>
-        <v>40604921.724999994</v>
+        <v>32259999.999999996</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.15">
@@ -1914,23 +1914,23 @@
       </c>
       <c r="D63" s="49">
         <f t="shared" si="22"/>
-        <v>13265646.802494032</v>
+        <v>13445008.460236887</v>
       </c>
       <c r="E63" s="49">
         <f t="shared" si="22"/>
-        <v>11783631.407502372</v>
+        <v>11374795.651638653</v>
       </c>
       <c r="F63" s="49">
         <f t="shared" si="22"/>
-        <v>10467208.437404457</v>
+        <v>9623346.574990401</v>
       </c>
       <c r="G63" s="49">
         <f t="shared" si="22"/>
-        <v>9297871.7614164911</v>
+        <v>8141579.1666585468</v>
       </c>
       <c r="H63" s="49">
         <f>H60/(1+$H$12)^H18</f>
-        <v>11818274.354573885</v>
+        <v>9939318.9178002533</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.15">
@@ -1943,23 +1943,23 @@
       </c>
       <c r="D64" s="49">
         <f>C64+D63</f>
-        <v>-40974462.786547065</v>
+        <v>-40795101.128804214</v>
       </c>
       <c r="E64" s="49">
         <f t="shared" ref="E64:H64" si="23">D64+E63</f>
-        <v>-29190831.379044693</v>
+        <v>-29420305.477165561</v>
       </c>
       <c r="F64" s="49">
         <f t="shared" si="23"/>
-        <v>-18723622.941640235</v>
+        <v>-19796958.902175158</v>
       </c>
       <c r="G64" s="49">
         <f t="shared" si="23"/>
-        <v>-9425751.1802237444</v>
+        <v>-11655379.735516611</v>
       </c>
       <c r="H64" s="49">
         <f t="shared" si="23"/>
-        <v>2392523.1743501406</v>
+        <v>-1716060.8177163582</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.15">
@@ -1969,7 +1969,7 @@
       <c r="B66" s="24"/>
       <c r="C66" s="50">
         <f>C60+NPV($H$12,D60:H60)</f>
-        <v>2392523.174350135</v>
+        <v>-1716060.8177163675</v>
       </c>
       <c r="D66" s="15"/>
     </row>
@@ -1980,7 +1980,7 @@
       <c r="B67" s="26"/>
       <c r="C67" s="27">
         <f>IRR(C60:H60)</f>
-        <v>0.19979255448030542</v>
+        <v>0.16858705103377836</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.15">
@@ -1990,7 +1990,7 @@
       <c r="B68" s="26"/>
       <c r="C68" s="28">
         <f>F18 - F61/G60</f>
-        <v>3.265103227212562</v>
+        <v>3.4130449024063112</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.15">
@@ -2009,7 +2009,7 @@
       <c r="B70" s="31"/>
       <c r="C70" s="32">
         <f>-NPV($H$12,D60:H60)/C60</f>
-        <v>1.0441098514084406</v>
+        <v>0.96836177451118044</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>